<commit_message>
Before route change from node-link to ni-link
</commit_message>
<xml_diff>
--- a/station_in_config/Point.xlsx
+++ b/station_in_config/Point.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="855" windowWidth="9015" windowHeight="8100"/>
+    <workbookView xWindow="7770" yWindow="495" windowWidth="11310" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
     <t>Axis_1</t>
   </si>
   <si>
-    <t>Line_7</t>
+    <t>Line_7 Point_15</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -165,7 +165,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -466,10 +465,13 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -498,7 +500,7 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>-1050</v>
       </c>
     </row>
@@ -512,7 +514,7 @@
       <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>900</v>
       </c>
     </row>
@@ -526,7 +528,7 @@
       <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>600</v>
       </c>
     </row>
@@ -540,7 +542,7 @@
       <c r="C5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>-950</v>
       </c>
     </row>
@@ -554,7 +556,7 @@
       <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>-800</v>
       </c>
     </row>
@@ -568,7 +570,7 @@
       <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>-450</v>
       </c>
     </row>
@@ -582,7 +584,7 @@
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>600</v>
       </c>
     </row>
@@ -596,7 +598,7 @@
       <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>700</v>
       </c>
     </row>
@@ -610,7 +612,7 @@
       <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>800</v>
       </c>
     </row>
@@ -624,7 +626,7 @@
       <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>-550</v>
       </c>
     </row>
@@ -638,7 +640,7 @@
       <c r="C12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>500</v>
       </c>
     </row>
@@ -652,7 +654,7 @@
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>-700</v>
       </c>
     </row>
@@ -666,7 +668,7 @@
       <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>350</v>
       </c>
     </row>
@@ -680,12 +682,12 @@
       <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -694,7 +696,7 @@
       <c r="D16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>500</v>
       </c>
     </row>
@@ -708,7 +710,7 @@
       <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>-900</v>
       </c>
     </row>
@@ -722,7 +724,7 @@
       <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>-750</v>
       </c>
     </row>
@@ -736,7 +738,7 @@
       <c r="C19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>650</v>
       </c>
     </row>
@@ -750,7 +752,7 @@
       <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>750</v>
       </c>
     </row>
@@ -764,7 +766,7 @@
       <c r="C21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>400</v>
       </c>
     </row>

</xml_diff>